<commit_message>
Se agrego el documento con los integrntes del grupo XD
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>nombre</t>
   </si>
@@ -27,103 +27,115 @@
     <t>existencia</t>
   </si>
   <si>
+    <t>Zapatos</t>
+  </si>
+  <si>
+    <t>Coca Cola</t>
+  </si>
+  <si>
+    <t>Computadora</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Gorras</t>
+  </si>
+  <si>
+    <t>Ropero</t>
+  </si>
+  <si>
+    <t>Manzanas</t>
+  </si>
+  <si>
+    <t>Jocotes</t>
+  </si>
+  <si>
+    <t>Hamburguesas XD</t>
+  </si>
+  <si>
+    <t>Waifus</t>
+  </si>
+  <si>
+    <t>Te Frio</t>
+  </si>
+  <si>
+    <t>nit</t>
+  </si>
+  <si>
+    <t>dirección</t>
+  </si>
+  <si>
+    <t>Cristian Alvarez</t>
+  </si>
+  <si>
+    <t>454227001-4</t>
+  </si>
+  <si>
+    <t>Aldea El Juez</t>
+  </si>
+  <si>
+    <t>Yossy Marroquín</t>
+  </si>
+  <si>
+    <t>134679852</t>
+  </si>
+  <si>
+    <t>Sansare</t>
+  </si>
+  <si>
+    <t>Melvin Cortéz</t>
+  </si>
+  <si>
+    <t>789456123</t>
+  </si>
+  <si>
+    <t>Jalapa</t>
+  </si>
+  <si>
+    <t>Faizal Arana</t>
+  </si>
+  <si>
+    <t>123789456</t>
+  </si>
+  <si>
+    <t>Dubai XD</t>
+  </si>
+  <si>
+    <t>Donald Gonz ;v</t>
+  </si>
+  <si>
+    <t>456321789</t>
+  </si>
+  <si>
+    <t>Manolo Sandoval</t>
+  </si>
+  <si>
+    <t>789654123</t>
+  </si>
+  <si>
+    <t>Marco Valdez</t>
+  </si>
+  <si>
+    <t>c/f</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>nombre cliente</t>
+  </si>
+  <si>
+    <t>nombre producto</t>
+  </si>
+  <si>
+    <t>cantidad producto</t>
+  </si>
+  <si>
+    <t>valor pedido</t>
+  </si>
+  <si>
     <t>Aguacate</t>
-  </si>
-  <si>
-    <t>Zapatos</t>
-  </si>
-  <si>
-    <t>Coca Cola</t>
-  </si>
-  <si>
-    <t>Computadora</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>Gorras</t>
-  </si>
-  <si>
-    <t>Ropero</t>
-  </si>
-  <si>
-    <t>Manzanas</t>
-  </si>
-  <si>
-    <t>Jocotes</t>
-  </si>
-  <si>
-    <t>Hamburguesas XD</t>
-  </si>
-  <si>
-    <t>Waifus</t>
-  </si>
-  <si>
-    <t>nit</t>
-  </si>
-  <si>
-    <t>dirección</t>
-  </si>
-  <si>
-    <t>Manolo Sandoval</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>Aldea El Juez</t>
-  </si>
-  <si>
-    <t>Cristian Alvarez</t>
-  </si>
-  <si>
-    <t>454227001-4</t>
-  </si>
-  <si>
-    <t>Yossy Marroquín</t>
-  </si>
-  <si>
-    <t>134679852</t>
-  </si>
-  <si>
-    <t>Sansare</t>
-  </si>
-  <si>
-    <t>Melvin Cortéz</t>
-  </si>
-  <si>
-    <t>789456123</t>
-  </si>
-  <si>
-    <t>Jalapa</t>
-  </si>
-  <si>
-    <t>Faizal Arana</t>
-  </si>
-  <si>
-    <t>123789456</t>
-  </si>
-  <si>
-    <t>Dubai XD</t>
-  </si>
-  <si>
-    <t>Donald Gonz ;v</t>
-  </si>
-  <si>
-    <t>456321789</t>
-  </si>
-  <si>
-    <t>nombre cliente</t>
-  </si>
-  <si>
-    <t>nombre producto</t>
-  </si>
-  <si>
-    <t>cantidad producto</t>
-  </si>
-  <si>
-    <t>valor pedido</t>
   </si>
 </sst>
 </file>
@@ -477,10 +489,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>250</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -488,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -499,10 +511,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>2000</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -510,10 +522,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2000</v>
+        <v>2750</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -521,10 +533,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2750</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -532,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>1300</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -543,10 +555,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1300</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -554,10 +566,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -565,10 +577,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1.5</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -576,10 +588,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -587,10 +599,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +612,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,40 +648,40 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -680,7 +692,18 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +713,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -698,24 +721,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -726,10 +749,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -740,10 +763,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -754,10 +777,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -768,10 +791,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -782,16 +805,30 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
         <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>